<commit_message>
replaced file for selenium test and fixed file validation
</commit_message>
<xml_diff>
--- a/t/data/cross/crosses_plots_upload_selenium.xlsx
+++ b/t/data/cross/crosses_plots_upload_selenium.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t xml:space="preserve">cross_unique_id</t>
   </si>
@@ -39,12 +39,6 @@
     <t xml:space="preserve">male_parent</t>
   </si>
   <si>
-    <t xml:space="preserve">female_plot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">male_plot</t>
-  </si>
-  <si>
     <t xml:space="preserve">test_cross_upload5</t>
   </si>
   <si>
@@ -52,12 +46,6 @@
   </si>
   <si>
     <t xml:space="preserve">biparental</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UG120001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UG120002</t>
   </si>
   <si>
     <t xml:space="preserve">KASESE_TP2013_842</t>
@@ -179,21 +167,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -212,57 +199,39 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -287,7 +256,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -310,7 +279,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>